<commit_message>
LA SEGUNDA CAPTURA  EN EL PPT INSERCION DE NOMBRES , EN EL XLSX SACAMOS MEDIDAS ESTADISTICAS + INSERCION DE VARIABLE  LUGAR ,  EN EL TXT  CONVERSACION 2 DE FAVORITE
</commit_message>
<xml_diff>
--- a/edad.xlsx
+++ b/edad.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>integrantes</t>
   </si>
@@ -37,6 +37,24 @@
   </si>
   <si>
     <t>jesus</t>
+  </si>
+  <si>
+    <t>Sacaremos el promedio de las edades de los alumnos</t>
+  </si>
+  <si>
+    <t>lugar de residencia</t>
+  </si>
+  <si>
+    <t>lima</t>
+  </si>
+  <si>
+    <t>cañete</t>
+  </si>
+  <si>
+    <t>ica</t>
+  </si>
+  <si>
+    <t>la moda de lugar de residencia es  :</t>
   </si>
 </sst>
 </file>
@@ -52,12 +70,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -87,12 +111,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,55 +398,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:D8"/>
+  <dimension ref="C4:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1">
         <v>22</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="3">
+        <f>SUM(D5+D6+D7+D8)/4</f>
+        <v>21.25</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>